<commit_message>
Changes the activate , deactivate, archive, restore, db_action methods, and implemented for the user module, for the database testing and client module data base testing
</commit_message>
<xml_diff>
--- a/ExcelData/TC_Leave.xlsx
+++ b/ExcelData/TC_Leave.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23370" windowHeight="10740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="10740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>leaveTypeName</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>30-August-2023</t>
+  </si>
+  <si>
+    <t>orgName</t>
+  </si>
+  <si>
+    <t>Westwood</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,7 +389,7 @@
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,8 +405,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -415,6 +424,9 @@
       </c>
       <c r="E2" t="s">
         <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>